<commit_message>
Add calculations to workbook
</commit_message>
<xml_diff>
--- a/code/Discrete State Space Example.xlsx
+++ b/code/Discrete State Space Example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianbaltser/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianbaltser/Documents/GitHub/master-thesis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C8EA4-AF46-0848-A1A2-B1C13FAAB693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DCE642-3C84-DD4F-98EA-71285AF3B620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="24000" windowHeight="37900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="riskfree_rate" localSheetId="2">'Example (2)'!$D$41</definedName>
     <definedName name="riskfree_rate">Initial!$D$26</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Example!$H$15</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Example (2)'!$Q$29</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Example (2)'!$J$29</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Initial!#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
@@ -74,7 +74,7 @@
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Example!$I$36</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Example (2)'!$R$43</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Example (2)'!$J$43</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Initial!#REF!</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
@@ -312,8 +312,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="77">
   <si>
     <t>State</t>
   </si>
@@ -511,13 +533,46 @@
   </si>
   <si>
     <t>Promised Yield</t>
+  </si>
+  <si>
+    <t>Theoretical Price</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>FVA (1)</t>
+  </si>
+  <si>
+    <t>DVA</t>
+  </si>
+  <si>
+    <t>EPE</t>
+  </si>
+  <si>
+    <t>Credit Spread</t>
+  </si>
+  <si>
+    <t>Loss Given Default</t>
+  </si>
+  <si>
+    <t>DVA2</t>
+  </si>
+  <si>
+    <t>XVAs</t>
+  </si>
+  <si>
+    <t>Risk Free Price</t>
+  </si>
+  <si>
+    <t>FVA (2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="12">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -527,6 +582,9 @@
     <numFmt numFmtId="169" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="0.000000000"/>
     <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.00000%"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -565,7 +623,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,12 +663,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,7 +761,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -880,8 +932,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -911,18 +961,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1330,8 +1407,8 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" s="9"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1645,10 +1722,10 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="87"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="3">
         <f>SUMPRODUCT($E$4:$E$8,D17:D21)</f>
         <v>0.98000000000000009</v>
@@ -1674,10 +1751,10 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="87"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="4">
         <f>SUMPRODUCT(D17:D21,$D$4:$D$8)/D24-1</f>
         <v>2.0408163265305923E-2</v>
@@ -1696,11 +1773,11 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="85" t="s">
+      <c r="A26" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="85"/>
-      <c r="C26" s="85"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="4">
         <f>D14/D24-1</f>
         <v>2.0408163265305923E-2</v>
@@ -1715,27 +1792,27 @@
       <c r="G26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="86" t="s">
+      <c r="I26" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="86"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="86"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="84"/>
+      <c r="L26" s="84"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="85" t="s">
+      <c r="A27" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="85"/>
-      <c r="C27" s="85"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
       <c r="F27" s="4">
         <f>IFERROR(LN(F14/F24), 0)</f>
         <v>8.0667903067454708E-2</v>
       </c>
-      <c r="I27" s="86"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="86"/>
-      <c r="L27" s="86"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="84"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E28" s="13" t="s">
@@ -1747,10 +1824,10 @@
       <c r="G28" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="86"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
-      <c r="L28" s="86"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84"/>
+      <c r="L28" s="84"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E29" s="19">
@@ -1765,10 +1842,10 @@
         <f>E29-F29</f>
         <v>3.8999999999999915</v>
       </c>
-      <c r="I29" s="86"/>
-      <c r="J29" s="86"/>
-      <c r="K29" s="86"/>
-      <c r="L29" s="86"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="84"/>
+      <c r="K29" s="84"/>
+      <c r="L29" s="84"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F30" s="20" t="s">
@@ -1864,8 +1941,8 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C1" s="9"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2015,10 +2092,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="88"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="27" t="s">
@@ -2045,11 +2122,11 @@
       <c r="H14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="88" t="s">
+      <c r="J14" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="27" t="s">
@@ -2063,9 +2140,9 @@
         <f>C15</f>
         <v>14.927071757421812</v>
       </c>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="29" t="s">
@@ -2081,9 +2158,9 @@
       <c r="H16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G17" s="13" t="s">
@@ -2311,10 +2388,10 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="87"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="3">
         <f t="shared" ref="D28:I28" si="5">SUMPRODUCT($E$4:$E$8,D21:D25)</f>
         <v>0.98000000000000009</v>
@@ -2348,10 +2425,10 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="87"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="4">
         <f>SUMPRODUCT(D21:D25,$D$4:$D$8)/D28-1</f>
         <v>2.0408163265305923E-2</v>
@@ -2378,11 +2455,11 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="85"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="4">
         <f>D18/D28-1</f>
         <v>2.0408163265305923E-2</v>
@@ -2404,19 +2481,19 @@
       <c r="I30" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="86" t="s">
+      <c r="K30" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="86"/>
-      <c r="M30" s="86"/>
-      <c r="N30" s="86"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="84"/>
+      <c r="N30" s="84"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="85" t="s">
+      <c r="A31" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
       <c r="G31" s="4">
         <f>IFERROR(LN(debt_face_value/G28), 0)</f>
         <v>7.3424625566442581E-2</v>
@@ -2425,20 +2502,20 @@
         <f>IFERROR(LN(H18/H28), 0)</f>
         <v>7.3424625566442775E-2</v>
       </c>
-      <c r="K31" s="86"/>
-      <c r="L31" s="86"/>
-      <c r="M31" s="86"/>
-      <c r="N31" s="86"/>
+      <c r="K31" s="84"/>
+      <c r="L31" s="84"/>
+      <c r="M31" s="84"/>
+      <c r="N31" s="84"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="86"/>
-      <c r="M32" s="86"/>
-      <c r="N32" s="86"/>
+      <c r="K32" s="84"/>
+      <c r="L32" s="84"/>
+      <c r="M32" s="84"/>
+      <c r="N32" s="84"/>
     </row>
     <row r="33" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
@@ -2455,10 +2532,10 @@
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="86"/>
-      <c r="M33" s="86"/>
-      <c r="N33" s="86"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="84"/>
+      <c r="M33" s="84"/>
+      <c r="N33" s="84"/>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.2">
       <c r="G34" s="20"/>
@@ -2520,7 +2597,7 @@
   <dimension ref="A1:T64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="151" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="E8" sqref="D8:E8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2535,8 +2612,8 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C1" s="9"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -2736,43 +2813,43 @@
       <c r="E13" s="48"/>
       <c r="F13" s="48"/>
       <c r="G13" s="49"/>
-      <c r="H13" s="92" t="s">
+      <c r="H13" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="92" t="s">
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="93"/>
-      <c r="N13" s="93"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="92" t="s">
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="91"/>
+      <c r="P13" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="94"/>
+      <c r="Q13" s="90"/>
+      <c r="R13" s="90"/>
+      <c r="S13" s="91"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G14" s="28"/>
-      <c r="H14" s="91" t="s">
+      <c r="H14" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="90"/>
+      <c r="I14" s="88"/>
       <c r="J14" s="41"/>
       <c r="K14" s="28"/>
-      <c r="L14" s="91" t="s">
+      <c r="L14" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="90"/>
+      <c r="M14" s="88"/>
       <c r="N14" s="41"/>
       <c r="O14" s="28"/>
-      <c r="P14" s="91" t="s">
+      <c r="P14" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="Q14" s="90"/>
+      <c r="Q14" s="88"/>
       <c r="R14" s="41"/>
       <c r="S14" s="28"/>
     </row>
@@ -2811,8 +2888,12 @@
       <c r="I16" s="44">
         <v>1</v>
       </c>
-      <c r="J16" s="41"/>
-      <c r="K16" s="28"/>
+      <c r="J16" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>67</v>
+      </c>
       <c r="L16" s="41" t="s">
         <v>46</v>
       </c>
@@ -2839,12 +2920,18 @@
       <c r="H17" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="44">
-        <f>I16/(1+0.008 + riskfree_rate)</f>
-        <v>0.97237656770916037</v>
-      </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="28"/>
+      <c r="I17" s="95">
+        <f>I16/(1 + I18 + riskfree_rate)</f>
+        <v>0.96116123970184408</v>
+      </c>
+      <c r="J17" s="41">
+        <f>SUM(E4:E8)*I16</f>
+        <v>0.98000000000000009</v>
+      </c>
+      <c r="K17" s="109">
+        <f>J17-I17</f>
+        <v>1.883876029815601E-2</v>
+      </c>
       <c r="L17" s="41" t="s">
         <v>44</v>
       </c>
@@ -2865,7 +2952,7 @@
         <f>SUMPRODUCT(P20:P24,E4:E8)</f>
         <v>0.9789000000000001</v>
       </c>
-      <c r="S17" s="81">
+      <c r="S17" s="79">
         <f>R17-Q17</f>
         <v>6.5234322908397369E-3</v>
       </c>
@@ -2876,8 +2963,7 @@
         <v>47</v>
       </c>
       <c r="I18" s="31">
-        <f>IFERROR(I16/I17-1-riskfree_rate, 0)</f>
-        <v>8.0000000000000071E-3</v>
+        <v>0.02</v>
       </c>
       <c r="J18" s="41"/>
       <c r="K18" s="28"/>
@@ -2897,11 +2983,11 @@
         <f>IFERROR(Q16/Q17-1-riskfree_rate, 0)</f>
         <v>8.0000000000000071E-3</v>
       </c>
-      <c r="R18" s="82">
+      <c r="R18" s="80">
         <f>Q16/(1+riskfree_rate+0.003)</f>
         <v>0.9771272458970629</v>
       </c>
-      <c r="S18" s="81">
+      <c r="S18" s="79">
         <f>R18-Q17</f>
         <v>4.750678187902535E-3</v>
       </c>
@@ -3021,8 +3107,9 @@
       <c r="I25" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="78">
-        <v>0.98</v>
+      <c r="J25" s="93">
+        <f>I17</f>
+        <v>0.96116123970184408</v>
       </c>
       <c r="K25" s="28"/>
       <c r="M25" t="s">
@@ -3046,8 +3133,9 @@
       <c r="I26" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="79">
-        <v>0.01</v>
+      <c r="J26" s="94">
+        <f>J29/J25-1-riskfree_rate</f>
+        <v>2.9095958173517067E-2</v>
       </c>
       <c r="K26" s="28"/>
       <c r="M26" s="13" t="s">
@@ -3124,14 +3212,14 @@
         <v>1</v>
       </c>
       <c r="F29" s="54">
-        <v>72.582228195153007</v>
+        <v>80</v>
       </c>
       <c r="G29" s="60"/>
       <c r="I29" s="54">
         <v>80</v>
       </c>
       <c r="J29" s="61">
-        <v>1.0205265585834735</v>
+        <v>1.0087426824343337</v>
       </c>
       <c r="K29" s="60"/>
       <c r="M29" s="54">
@@ -3269,11 +3357,11 @@
       </c>
       <c r="F32" s="51">
         <f>MIN(debt_face_value,E32)</f>
-        <v>72.582228195153007</v>
+        <v>80</v>
       </c>
       <c r="G32" s="55">
         <f>MAX(0,E32-F32)</f>
-        <v>47.417771804846993</v>
+        <v>40</v>
       </c>
       <c r="H32" s="56">
         <f>$E32+I$16</f>
@@ -3285,11 +3373,11 @@
       </c>
       <c r="J32" s="73">
         <f>IF(H32&gt;I$29+J$29, J$29, H32*((J$29)/(J$29+I$29)))</f>
-        <v>1.0205265585834735</v>
+        <v>1.0087426824343337</v>
       </c>
       <c r="K32" s="58">
         <f>MAX(0,H32-J32-I32)</f>
-        <v>39.97947344141653</v>
+        <v>39.991257317565669</v>
       </c>
       <c r="L32" s="56">
         <f>$E32+$I$16</f>
@@ -3337,11 +3425,11 @@
       </c>
       <c r="F33" s="51">
         <f>MIN(debt_face_value,E33)</f>
-        <v>72.582228195153007</v>
+        <v>80</v>
       </c>
       <c r="G33" s="55">
         <f t="shared" ref="G33:G36" si="2">MAX(0,E33-F33)</f>
-        <v>37.417771804846993</v>
+        <v>30</v>
       </c>
       <c r="H33" s="56">
         <f t="shared" ref="H33:H36" si="3">$E33+I$16</f>
@@ -3353,11 +3441,11 @@
       </c>
       <c r="J33" s="73">
         <f t="shared" ref="J33:J36" si="5">IF(H33&gt;I$29+J$29, J$29, H33*((J$29)/(J$29+I$29)))</f>
-        <v>1.0205265585834735</v>
+        <v>1.0087426824343337</v>
       </c>
       <c r="K33" s="58">
         <f t="shared" ref="K33:K36" si="6">MAX(0,H33-J33-I33)</f>
-        <v>29.97947344141653</v>
+        <v>29.991257317565669</v>
       </c>
       <c r="L33" s="56">
         <f t="shared" ref="L33:L36" si="7">$E33+$I$16</f>
@@ -3405,11 +3493,11 @@
       </c>
       <c r="F34" s="51">
         <f>MIN(debt_face_value,E34)</f>
-        <v>72.582228195153007</v>
+        <v>80</v>
       </c>
       <c r="G34" s="55">
         <f t="shared" si="2"/>
-        <v>27.417771804846993</v>
+        <v>20</v>
       </c>
       <c r="H34" s="56">
         <f t="shared" si="3"/>
@@ -3421,11 +3509,11 @@
       </c>
       <c r="J34" s="73">
         <f t="shared" si="5"/>
-        <v>1.0205265585834735</v>
+        <v>1.0087426824343337</v>
       </c>
       <c r="K34" s="58">
         <f t="shared" si="6"/>
-        <v>19.97947344141653</v>
+        <v>19.991257317565669</v>
       </c>
       <c r="L34" s="56">
         <f t="shared" si="7"/>
@@ -3473,11 +3561,11 @@
       </c>
       <c r="F35" s="51">
         <f>MIN(debt_face_value,E35)</f>
-        <v>72.582228195153007</v>
+        <v>80</v>
       </c>
       <c r="G35" s="55">
         <f t="shared" si="2"/>
-        <v>22.417771804846993</v>
+        <v>15</v>
       </c>
       <c r="H35" s="56">
         <f t="shared" si="3"/>
@@ -3489,11 +3577,11 @@
       </c>
       <c r="J35" s="73">
         <f t="shared" si="5"/>
-        <v>1.0205265585834735</v>
+        <v>1.0087426824343337</v>
       </c>
       <c r="K35" s="58">
         <f t="shared" si="6"/>
-        <v>14.97947344141653</v>
+        <v>14.991257317565669</v>
       </c>
       <c r="L35" s="56">
         <f t="shared" si="7"/>
@@ -3552,12 +3640,12 @@
         <v>61</v>
       </c>
       <c r="I36" s="51">
-        <f t="shared" si="4"/>
-        <v>60.231650018608818</v>
+        <f>IF(H36&gt;I$29+J$29, I$29, H36*((I$29)/(J$29+I$29)))</f>
+        <v>60.240411570517601</v>
       </c>
       <c r="J36" s="73">
-        <f t="shared" si="5"/>
-        <v>0.76834998139118826</v>
+        <f>IF(H36&gt;I$29+J$29, J$29, H36*((J$29)/(J$29+I$29)))</f>
+        <v>0.75958842948240246</v>
       </c>
       <c r="K36" s="58">
         <f t="shared" si="6"/>
@@ -3653,44 +3741,44 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="87"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="51">
         <f>SUMPRODUCT($E$4:$E$8,D32:D36)</f>
         <v>0.98000000000000009</v>
       </c>
-      <c r="E39" s="51">
-        <f t="shared" ref="D39:S39" si="13">SUMPRODUCT($E$4:$E$8,E32:E36)</f>
+      <c r="E39" s="73">
+        <f>SUMPRODUCT($E$4:$E$8,E32:E36)</f>
         <v>96.15</v>
       </c>
-      <c r="F39" s="51">
-        <f t="shared" si="13"/>
-        <v>69.746538529783123</v>
-      </c>
-      <c r="G39" s="55">
-        <f t="shared" si="13"/>
-        <v>26.403461470216882</v>
+      <c r="F39" s="73">
+        <f>SUMPRODUCT($E$4:$E$8,F32:F36)</f>
+        <v>76.199999999999989</v>
+      </c>
+      <c r="G39" s="58">
+        <f>SUMPRODUCT($E$4:$E$8,G32:G36)</f>
+        <v>19.950000000000003</v>
       </c>
       <c r="H39" s="51">
-        <f t="shared" si="13"/>
+        <f>SUMPRODUCT($E$4:$E$8,H32:H36)</f>
         <v>97.13</v>
       </c>
       <c r="I39" s="51">
-        <f t="shared" si="13"/>
-        <v>76.225481502046961</v>
+        <f>SUMPRODUCT($E$4:$E$8,I32:I36)</f>
+        <v>76.226445272756933</v>
       </c>
       <c r="J39" s="73">
-        <f t="shared" si="13"/>
-        <v>0.97237660392065273</v>
+        <f>SUMPRODUCT($E$4:$E$8,J32:J36)</f>
+        <v>0.96116086096093467</v>
       </c>
       <c r="K39" s="55">
-        <f t="shared" si="13"/>
-        <v>19.93214189403238</v>
+        <f>SUMPRODUCT($E$4:$E$8,K32:K36)</f>
+        <v>19.942393866282131</v>
       </c>
       <c r="L39" s="51">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="E39:S39" si="13">SUMPRODUCT($E$4:$E$8,L32:L36)</f>
         <v>97.13</v>
       </c>
       <c r="M39" s="51">
@@ -3723,10 +3811,10 @@
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="87" t="s">
+      <c r="B40" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="87"/>
+      <c r="C40" s="85"/>
       <c r="D40" s="50">
         <f>SUMPRODUCT(D32:D36,$D$4:$D$8)/D39-1</f>
         <v>2.0408163265305923E-2</v>
@@ -3737,11 +3825,11 @@
       </c>
       <c r="F40" s="50">
         <f>IFERROR(SUMPRODUCT(F32:F36,$D$4:$D$8)/F39 -1, 0)</f>
-        <v>3.1637100594891665E-2</v>
+        <v>3.6745406824147064E-2</v>
       </c>
       <c r="G40" s="62">
         <f>IFERROR(SUMPRODUCT(G32:G36,$D$4:$D$8)/G39-1, 0)</f>
-        <v>0.12852185112984316</v>
+        <v>0.14035087719298223</v>
       </c>
       <c r="H40" s="50">
         <f>SUMPRODUCT(H32:H36,$D$4:$D$8)/H39-1</f>
@@ -3749,15 +3837,15 @@
       </c>
       <c r="I40" s="50">
         <f>IFERROR(SUMPRODUCT(I32:I36,$D$4:$D$8)/I39 -1, 0)</f>
-        <v>3.6550782546498795E-2</v>
+        <v>3.6543423949542353E-2</v>
       </c>
       <c r="J40" s="50">
         <f>IFERROR(SUMPRODUCT(J32:J36,$D$4:$D$8)/J39 -1, 0)</f>
-        <v>3.6550782546498573E-2</v>
+        <v>3.6543423949542353E-2</v>
       </c>
       <c r="K40" s="62">
         <f>IFERROR(SUMPRODUCT(K32:K36,$D$4:$D$8)/K39-1, 0)</f>
-        <v>0.14039423812004603</v>
+        <v>0.14036933600725887</v>
       </c>
       <c r="L40" s="50">
         <f>SUMPRODUCT(L32:L36,$D$4:$D$8)/L39-1</f>
@@ -3793,11 +3881,11 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="83"/>
       <c r="D41" s="50">
         <f>D29/D39-1</f>
         <v>2.0408163265305923E-2</v>
@@ -3807,7 +3895,7 @@
       </c>
       <c r="F41" s="50">
         <f>IFERROR(debt_face_value/F39-1, 0)</f>
-        <v>4.0657066646526019E-2</v>
+        <v>4.9868766404199683E-2</v>
       </c>
       <c r="G41" s="43" t="s">
         <v>8</v>
@@ -3817,11 +3905,11 @@
       </c>
       <c r="I41" s="50">
         <f>IFERROR(debt_face_value/I39-1, 0)</f>
-        <v>-4.7795740152800748E-2</v>
+        <v>4.9504534990977955E-2</v>
       </c>
       <c r="J41" s="50">
         <f>IFERROR(J29/J39-1, 0)</f>
-        <v>4.9517804592046577E-2</v>
+        <v>4.9504534990977955E-2</v>
       </c>
       <c r="K41" s="43" t="s">
         <v>8</v>
@@ -3831,7 +3919,7 @@
       </c>
       <c r="M41" s="50">
         <f>IFERROR(debt_face_value/M39-1, 0)</f>
-        <v>0.48126996316638793</v>
+        <v>0.63265306122448983</v>
       </c>
       <c r="N41" s="50">
         <f>IFERROR(N29/N39-1, 0)</f>
@@ -3866,36 +3954,36 @@
       <c r="N42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="80"/>
+      <c r="R42" s="78"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F43" s="20"/>
       <c r="G43" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H43" s="45">
+      <c r="H43" s="107">
         <f>H39-$E$39</f>
         <v>0.97999999999998977</v>
       </c>
-      <c r="I43" s="45">
+      <c r="I43" s="108">
         <f>I39-$F$39</f>
-        <v>6.4789429722638374</v>
-      </c>
-      <c r="J43" s="67">
-        <f>J39-$I$17</f>
-        <v>3.6211492360216369E-8</v>
-      </c>
-      <c r="K43" s="45">
+        <v>2.644527275694486E-2</v>
+      </c>
+      <c r="J43" s="108">
+        <f>J39-I17</f>
+        <v>-3.7874090941247829E-7</v>
+      </c>
+      <c r="K43" s="108">
         <f>K39-$G$39</f>
-        <v>-6.4713195761845022</v>
+        <v>-7.6061337178714439E-3</v>
       </c>
       <c r="L43" s="45">
         <f>L39-I39</f>
-        <v>20.904518497953035</v>
+        <v>20.903554727243062</v>
       </c>
       <c r="M43" s="45">
         <f>M39-F39</f>
-        <v>-20.746538529783123</v>
+        <v>-27.199999999999989</v>
       </c>
       <c r="N43" s="24">
         <f>N39-D39*N25</f>
@@ -3903,7 +3991,7 @@
       </c>
       <c r="O43" s="45">
         <f>O39-G39</f>
-        <v>8.0065525297831215</v>
+        <v>14.460014000000001</v>
       </c>
       <c r="P43" s="68">
         <f>P39-$E$39</f>
@@ -3911,27 +3999,24 @@
       </c>
       <c r="Q43" s="68">
         <f>Q39-$F$39</f>
-        <v>1.6810001512283179E-2</v>
+        <v>-6.4366514687045822</v>
       </c>
       <c r="R43" s="67">
         <f>R39-Q17</f>
         <v>-3.4317400354755279E-7</v>
       </c>
-      <c r="S43" s="83">
+      <c r="S43" s="81">
         <f>S39-$G$39</f>
-        <v>-1.028622604744811E-2</v>
+        <v>6.4431752441694314</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F44" s="20"/>
       <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="22">
-        <f>(J41-(riskfree_rate+0.02))^2</f>
-        <v>8.2985565101861158E-5</v>
-      </c>
-      <c r="K44" s="15"/>
+      <c r="H44" s="98"/>
+      <c r="I44" s="105"/>
+      <c r="J44" s="105"/>
+      <c r="K44" s="106"/>
       <c r="L44" s="40"/>
       <c r="M44" s="20"/>
       <c r="N44" s="22"/>
@@ -3947,14 +4032,14 @@
       </c>
       <c r="G45" s="63">
         <f>SUMPRODUCT(F39:G39,F40:G40)/(E39)</f>
-        <v>5.8242329693187718E-2</v>
+        <v>5.8242329693187739E-2</v>
       </c>
       <c r="H45" s="64"/>
       <c r="I45" s="64"/>
       <c r="J45" s="64"/>
       <c r="K45" s="65">
         <f>SUMPRODUCT(I39:K39, I40:K40)/H39</f>
-        <v>5.7860599196952731E-2</v>
+        <v>5.7860599196952571E-2</v>
       </c>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
@@ -3977,14 +4062,14 @@
       </c>
       <c r="G46" s="51">
         <f>G45*E39</f>
-        <v>5.6</v>
+        <v>5.6000000000000014</v>
       </c>
       <c r="H46" s="23"/>
       <c r="I46" s="52"/>
       <c r="J46" s="53"/>
       <c r="K46" s="51">
         <f>K45*H39</f>
-        <v>5.6200000000000188</v>
+        <v>5.6200000000000028</v>
       </c>
       <c r="M46" s="39"/>
       <c r="N46" s="21"/>
@@ -4003,38 +4088,58 @@
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I47" s="39"/>
       <c r="J47" s="21"/>
+      <c r="K47" s="97">
+        <f>K45-G45</f>
+        <v>-3.817304962351678E-4</v>
+      </c>
       <c r="M47" s="39"/>
       <c r="N47" s="21"/>
       <c r="Q47" s="39"/>
       <c r="R47" s="21"/>
       <c r="S47" s="66">
         <f>S46-G46</f>
-        <v>2.0600000000009722E-2</v>
+        <v>2.0600000000007945E-2</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E48" s="88" t="s">
+      <c r="E48" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="88"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="86"/>
       <c r="H48" s="14"/>
+      <c r="K48" s="66">
+        <f>K46-G46</f>
+        <v>2.000000000000135E-2</v>
+      </c>
       <c r="L48" s="14"/>
       <c r="P48" s="14"/>
     </row>
     <row r="49" spans="5:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E49" s="88"/>
-      <c r="F49" s="88"/>
-      <c r="G49" s="88"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="86"/>
+      <c r="G49" s="86"/>
       <c r="H49" s="14"/>
+      <c r="K49" s="47">
+        <f>SUM(F4:F7)*J50</f>
+        <v>2.4330685105245175E-2</v>
+      </c>
       <c r="L49" s="14"/>
       <c r="P49" s="14"/>
     </row>
     <row r="50" spans="5:20" x14ac:dyDescent="0.2">
-      <c r="E50" s="88"/>
-      <c r="F50" s="88"/>
-      <c r="G50" s="88"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="86"/>
+      <c r="G50" s="86"/>
       <c r="H50" s="14"/>
+      <c r="I50" s="102" t="s">
+        <v>68</v>
+      </c>
+      <c r="J50" s="67">
+        <f>J25*(J41-riskfree_rate)*D39</f>
+        <v>2.7406978624299166E-2</v>
+      </c>
+      <c r="K50" s="67"/>
       <c r="L50" s="14"/>
       <c r="P50" s="69"/>
       <c r="Q50" s="69"/>
@@ -4042,37 +4147,118 @@
       <c r="S50" s="69"/>
     </row>
     <row r="51" spans="5:20" x14ac:dyDescent="0.2">
-      <c r="E51" s="88"/>
-      <c r="F51" s="88"/>
-      <c r="G51" s="88"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
       <c r="H51" s="14"/>
+      <c r="I51" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="J51" s="101">
+        <f>J29</f>
+        <v>1.0087426824343337</v>
+      </c>
+      <c r="K51" s="99"/>
       <c r="L51" s="14"/>
       <c r="P51" s="14"/>
     </row>
     <row r="52" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <f>F29/(1+riskfree_rate)</f>
+        <v>78.40000000000002</v>
+      </c>
+      <c r="I52" t="s">
+        <v>72</v>
+      </c>
+      <c r="J52" s="67" cm="1">
+        <f t="array" ref="J52">SUM((1-J32:J36/J29) * F4:F8)</f>
+        <v>2.7723912337283978E-2</v>
+      </c>
+      <c r="K52" s="99"/>
       <c r="Q52" s="47"/>
       <c r="R52" s="47"/>
       <c r="S52" s="47"/>
     </row>
     <row r="53" spans="5:20" x14ac:dyDescent="0.2">
-      <c r="J53" s="25"/>
+      <c r="E53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53">
+        <f>(1-F36/F29)*D39*F29*F8</f>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="I53" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="J53" s="67">
+        <f>J52*D39*J51</f>
+        <v>2.7406967824712438E-2</v>
+      </c>
+      <c r="K53" s="67"/>
       <c r="N53" s="25"/>
       <c r="Q53" s="47"/>
       <c r="R53" s="47"/>
       <c r="S53" s="47"/>
     </row>
     <row r="54" spans="5:20" x14ac:dyDescent="0.2">
-      <c r="J54" s="25"/>
+      <c r="E54" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="96">
+        <f>(1+riskfree_rate) * ((F8*(1-F36/F29))/(1-F8*(1-F36/F29)))</f>
+        <v>2.946060313889334E-2</v>
+      </c>
+      <c r="J54" s="67"/>
       <c r="N54" s="25"/>
       <c r="R54" s="25"/>
     </row>
+    <row r="55" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <f>F29/(1+F54+riskfree_rate)</f>
+        <v>76.200000000000017</v>
+      </c>
+      <c r="I55" t="s">
+        <v>75</v>
+      </c>
+      <c r="J55" s="67">
+        <f>J29/(1 + riskfree_rate)</f>
+        <v>0.98856782878564731</v>
+      </c>
+    </row>
+    <row r="56" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="I56" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="J56" s="67">
+        <f>J55-J39</f>
+        <v>2.7406967824712636E-2</v>
+      </c>
+      <c r="K56" s="67"/>
+    </row>
+    <row r="58" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="I58" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="J58" s="67">
+        <f>D39 * (D39 * J29) * (J41-riskfree_rate) * SUM(F4:F7)</f>
+        <v>2.5024451209477293E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="J59" s="67">
+        <f>K43/SUM(F4:F7)</f>
+        <v>-8.5678287856482942E-3</v>
+      </c>
+    </row>
     <row r="60" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="J60" s="99"/>
       <c r="Q60" s="47"/>
       <c r="R60" s="47"/>
       <c r="S60" s="47"/>
       <c r="T60" s="77"/>
     </row>
     <row r="61" spans="5:20" x14ac:dyDescent="0.2">
+      <c r="J61" s="99"/>
       <c r="Q61" s="47"/>
       <c r="R61" s="47"/>
       <c r="S61" s="47"/>
@@ -4083,17 +4269,17 @@
     <row r="64" spans="5:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A41:C41"/>
     <mergeCell ref="E48:G51"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="L13:O13"/>
     <mergeCell ref="P13:S13"/>
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="L14:M14"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A41:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>